<commit_message>
Fixed Easy enemy bug
</commit_message>
<xml_diff>
--- a/data/EnemyTemplates.xlsx
+++ b/data/EnemyTemplates.xlsx
@@ -1189,10 +1189,10 @@
   <dimension ref="A1:W112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V1:Y1048576"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1329,7 +1329,7 @@
         <v>00</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f>IF($C3="00",$C3,DEC2HEX(MAX(ROUND(HEX2DEC($C3)/3,0),1),2))</f>
+        <f>IF($C3="00",$C3,DEC2HEX(MAX(ROUND(HEX2DEC($C3)/9,0),1),2))</f>
         <v>00</v>
       </c>
       <c r="H3" s="4" t="str">
@@ -1410,7 +1410,7 @@
         <v>04</v>
       </c>
       <c r="G4" s="4" t="str">
-        <f t="shared" ref="G4:G67" si="1">IF($C4="00",$C4,DEC2HEX(MAX(ROUND(HEX2DEC($C4)/3,0),1),2))</f>
+        <f t="shared" ref="G4:G67" si="1">IF($C4="00",$C4,DEC2HEX(MAX(ROUND(HEX2DEC($C4)/9,0),1),2))</f>
         <v>01</v>
       </c>
       <c r="H4" s="4" t="str">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="G20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="G23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="G27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="G29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="G30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3871,7 +3871,7 @@
       </c>
       <c r="G33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4120,7 +4120,7 @@
       </c>
       <c r="G36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="G37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="G42" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H42" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="G43" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H43" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="G44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>04</v>
+        <v>01</v>
       </c>
       <c r="H44" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="G45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H45" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="G46" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H46" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="G47" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H47" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="G48" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H48" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="G49" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H49" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5299,7 +5299,7 @@
       </c>
       <c r="G50" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H50" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="G51" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H51" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="G52" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H52" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="G53" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H53" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="G54" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H54" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="G55" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H55" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="G56" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H56" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="G57" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H57" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="G58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H58" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="G59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H59" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6142,7 +6142,7 @@
       </c>
       <c r="G60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H60" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="G61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H61" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="G62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H62" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="G63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H63" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6478,7 +6478,7 @@
       </c>
       <c r="G64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H64" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="G65" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>06</v>
+        <v>02</v>
       </c>
       <c r="H65" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="G66" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H66" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="G67" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H67" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6819,8 +6819,8 @@
         <v>04</v>
       </c>
       <c r="G68" s="4" t="str">
-        <f t="shared" ref="G68:G112" si="17">IF($C68="00",$C68,DEC2HEX(MAX(ROUND(HEX2DEC($C68)/3,0),1),2))</f>
-        <v>03</v>
+        <f t="shared" ref="G68:G112" si="17">IF($C68="00",$C68,DEC2HEX(MAX(ROUND(HEX2DEC($C68)/9,0),1),2))</f>
+        <v>01</v>
       </c>
       <c r="H68" s="4" t="str">
         <f t="shared" ref="H68:H112" si="18">IF(OR($D68="7F",$D68="FF"),$D68,"00")</f>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="G69" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H69" s="4" t="str">
         <f t="shared" si="18"/>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="G70" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>09</v>
+        <v>03</v>
       </c>
       <c r="H70" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="G71" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H71" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7162,7 +7162,7 @@
       </c>
       <c r="G72" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H72" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="G73" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H73" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="G74" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H74" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="G75" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H75" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7498,7 +7498,7 @@
       </c>
       <c r="G76" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H76" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="G77" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H77" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="G78" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H78" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="G79" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H79" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="G80" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>09</v>
+        <v>03</v>
       </c>
       <c r="H80" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="G81" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H81" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8011,7 +8011,7 @@
       </c>
       <c r="G82" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>08</v>
+        <v>03</v>
       </c>
       <c r="H82" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="G83" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0B</v>
+        <v>04</v>
       </c>
       <c r="H83" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="G84" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>07</v>
+        <v>02</v>
       </c>
       <c r="H84" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="G85" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H85" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="G86" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="H86" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="G87" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H87" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8515,7 +8515,7 @@
       </c>
       <c r="G88" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H88" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8596,7 +8596,7 @@
       </c>
       <c r="G89" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0D</v>
+        <v>04</v>
       </c>
       <c r="H89" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="G90" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H90" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8758,7 +8758,7 @@
       </c>
       <c r="G91" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0E</v>
+        <v>05</v>
       </c>
       <c r="H91" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="G92" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>05</v>
+        <v>02</v>
       </c>
       <c r="H92" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8920,7 +8920,7 @@
       </c>
       <c r="G93" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H93" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9001,7 +9001,7 @@
       </c>
       <c r="G94" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H94" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9082,7 +9082,7 @@
       </c>
       <c r="G95" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H95" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="G96" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H96" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9244,7 +9244,7 @@
       </c>
       <c r="G97" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H97" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9325,7 +9325,7 @@
       </c>
       <c r="G98" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H98" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="G99" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H99" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9487,7 +9487,7 @@
       </c>
       <c r="G100" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H100" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9574,7 +9574,7 @@
       </c>
       <c r="G101" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H101" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9661,7 +9661,7 @@
       </c>
       <c r="G102" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0C</v>
+        <v>04</v>
       </c>
       <c r="H102" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9748,7 +9748,7 @@
       </c>
       <c r="G103" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="H103" s="4" t="str">
         <f t="shared" si="18"/>
@@ -10153,7 +10153,7 @@
       </c>
       <c r="G108" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>0D</v>
+        <v>04</v>
       </c>
       <c r="H108" s="4" t="str">
         <f t="shared" si="18"/>

</xml_diff>

<commit_message>
Addl functionality for Glasses and Ring
Also, brought Easy mode enemy STR up to Normal levels
</commit_message>
<xml_diff>
--- a/data/EnemyTemplates.xlsx
+++ b/data/EnemyTemplates.xlsx
@@ -1192,7 +1192,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G112"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1329,7 +1329,7 @@
         <v>00</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f>IF($C3="00",$C3,DEC2HEX(MAX(ROUND(HEX2DEC($C3)/9,0),1),2))</f>
+        <f>IF($C3="00",$C3,DEC2HEX(MAX(ROUND(HEX2DEC($C3)*7/30,0),1),2))</f>
         <v>00</v>
       </c>
       <c r="H3" s="4" t="str">
@@ -1410,7 +1410,7 @@
         <v>04</v>
       </c>
       <c r="G4" s="4" t="str">
-        <f t="shared" ref="G4:G67" si="1">IF($C4="00",$C4,DEC2HEX(MAX(ROUND(HEX2DEC($C4)/9,0),1),2))</f>
+        <f t="shared" ref="G4:G67" si="1">IF($C4="00",$C4,DEC2HEX(MAX(ROUND(HEX2DEC($C4)*7/30,0),1),2))</f>
         <v>01</v>
       </c>
       <c r="H4" s="4" t="str">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="G23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="G27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="G29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="G30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -3871,7 +3871,7 @@
       </c>
       <c r="G33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4120,7 +4120,7 @@
       </c>
       <c r="G36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="G37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="G42" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H42" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="G43" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H43" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="G44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>03</v>
       </c>
       <c r="H44" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="G45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H45" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="G46" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H46" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="G47" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H47" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="G48" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H48" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="G49" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H49" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5299,7 +5299,7 @@
       </c>
       <c r="G50" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H50" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="G51" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H51" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="G52" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H52" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="G53" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H53" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="G54" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H54" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="G55" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H55" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="G56" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H56" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="G57" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H57" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="G58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H58" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="G59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H59" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6142,7 +6142,7 @@
       </c>
       <c r="G60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H60" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="G61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H61" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="G62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H62" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="G63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H63" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6478,7 +6478,7 @@
       </c>
       <c r="G64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H64" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="G65" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>04</v>
       </c>
       <c r="H65" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="G66" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H66" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="G67" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H67" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6819,8 +6819,8 @@
         <v>04</v>
       </c>
       <c r="G68" s="4" t="str">
-        <f t="shared" ref="G68:G112" si="17">IF($C68="00",$C68,DEC2HEX(MAX(ROUND(HEX2DEC($C68)/9,0),1),2))</f>
-        <v>01</v>
+        <f t="shared" ref="G68:G112" si="17">IF($C68="00",$C68,DEC2HEX(MAX(ROUND(HEX2DEC($C68)*7/30,0),1),2))</f>
+        <v>02</v>
       </c>
       <c r="H68" s="4" t="str">
         <f t="shared" ref="H68:H112" si="18">IF(OR($D68="7F",$D68="FF"),$D68,"00")</f>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="G69" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H69" s="4" t="str">
         <f t="shared" si="18"/>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="G70" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>06</v>
       </c>
       <c r="H70" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="G71" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H71" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7162,7 +7162,7 @@
       </c>
       <c r="G72" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>06</v>
       </c>
       <c r="H72" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="G73" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H73" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="G74" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>05</v>
       </c>
       <c r="H74" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="G75" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H75" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7498,7 +7498,7 @@
       </c>
       <c r="G76" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>05</v>
       </c>
       <c r="H76" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="G77" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H77" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="G78" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H78" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="G79" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>05</v>
       </c>
       <c r="H79" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="G80" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>06</v>
       </c>
       <c r="H80" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="G81" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>06</v>
       </c>
       <c r="H81" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8011,7 +8011,7 @@
       </c>
       <c r="G82" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>03</v>
+        <v>05</v>
       </c>
       <c r="H82" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="G83" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H83" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="G84" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>05</v>
       </c>
       <c r="H84" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="G85" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H85" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="G86" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H86" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="G87" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H87" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8515,7 +8515,7 @@
       </c>
       <c r="G88" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H88" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8596,7 +8596,7 @@
       </c>
       <c r="G89" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>09</v>
       </c>
       <c r="H89" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="G90" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H90" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8758,7 +8758,7 @@
       </c>
       <c r="G91" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>05</v>
+        <v>0A</v>
       </c>
       <c r="H91" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="G92" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>02</v>
+        <v>03</v>
       </c>
       <c r="H92" s="4" t="str">
         <f t="shared" si="18"/>
@@ -8920,7 +8920,7 @@
       </c>
       <c r="G93" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H93" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9001,7 +9001,7 @@
       </c>
       <c r="G94" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H94" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9082,7 +9082,7 @@
       </c>
       <c r="G95" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H95" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="G96" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H96" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9244,7 +9244,7 @@
       </c>
       <c r="G97" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H97" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9325,7 +9325,7 @@
       </c>
       <c r="G98" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H98" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="G99" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H99" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9487,7 +9487,7 @@
       </c>
       <c r="G100" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H100" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9574,7 +9574,7 @@
       </c>
       <c r="G101" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H101" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9661,7 +9661,7 @@
       </c>
       <c r="G102" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="H102" s="4" t="str">
         <f t="shared" si="18"/>
@@ -9748,7 +9748,7 @@
       </c>
       <c r="G103" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="H103" s="4" t="str">
         <f t="shared" si="18"/>
@@ -10153,7 +10153,7 @@
       </c>
       <c r="G108" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>04</v>
+        <v>09</v>
       </c>
       <c r="H108" s="4" t="str">
         <f t="shared" si="18"/>

</xml_diff>

<commit_message>
v3.4.4 DEF works better now
</commit_message>
<xml_diff>
--- a/data/EnemyTemplates.xlsx
+++ b/data/EnemyTemplates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bravo Properties\Documents\Gaming\Illusion of Gaia Randomizer\IoGR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB544272-F39A-4B1B-8E0A-EB3523B00BCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A749B-E47E-493E-84DD-30581EBBDD79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="3855" windowWidth="28575" windowHeight="10365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatTable" sheetId="2" r:id="rId1"/>
@@ -1361,10 +1361,10 @@
   <dimension ref="A1:AE112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3:K112"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3:M112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1553,7 +1553,7 @@
         <v>00</v>
       </c>
       <c r="K3" s="4" t="str">
-        <f>IF($G3="00",$G3,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G3)+1.669,0),2),2))</f>
+        <f>IF($G3="00",$G3,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G3)+0.669,0),1),2))</f>
         <v>00</v>
       </c>
       <c r="L3" s="4" t="str">
@@ -1660,8 +1660,8 @@
         <v>02</v>
       </c>
       <c r="K4" s="4" t="str">
-        <f t="shared" ref="K4:K67" si="6">IF($G4="00",$G4,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G4)+1.669,0),2),2))</f>
-        <v>02</v>
+        <f t="shared" ref="K4:K67" si="6">IF($G4="00",$G4,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G4)+0.669,0),1),2))</f>
+        <v>01</v>
       </c>
       <c r="L4" s="4" t="str">
         <f t="shared" ref="L4:L67" si="7">IF(OR($H4="7F",$H4="FF"),$H4,"00")</f>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L5" s="4" t="str">
         <f t="shared" si="7"/>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L6" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L7" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L8" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2345,7 +2345,7 @@
       </c>
       <c r="K10" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L10" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="K11" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L11" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="K12" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L12" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L13" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="K14" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L14" s="4" t="str">
         <f t="shared" si="7"/>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="K15" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L15" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="K16" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L16" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L17" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="K18" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L18" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="K19" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L19" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L20" s="4" t="str">
         <f t="shared" si="7"/>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="K23" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L23" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4243,7 +4243,7 @@
       </c>
       <c r="K27" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L27" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="K28" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L28" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4473,7 +4473,7 @@
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L29" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="K30" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L30" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4703,7 +4703,7 @@
       </c>
       <c r="K31" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>06</v>
+        <v>05</v>
       </c>
       <c r="L31" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L32" s="4" t="str">
         <f t="shared" si="7"/>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>06</v>
+        <v>05</v>
       </c>
       <c r="L33" s="4" t="str">
         <f t="shared" si="7"/>
@@ -5048,7 +5048,7 @@
       </c>
       <c r="K34" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L34" s="4" t="str">
         <f t="shared" si="7"/>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L35" s="4" t="str">
         <f t="shared" si="7"/>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L36" s="4" t="str">
         <f t="shared" si="7"/>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="K37" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>06</v>
+        <v>05</v>
       </c>
       <c r="L37" s="4" t="str">
         <f t="shared" si="7"/>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="K42" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L42" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="K43" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L43" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="K44" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L44" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="K45" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L45" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6377,7 +6377,7 @@
       </c>
       <c r="K46" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L46" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="K47" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L47" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6607,7 +6607,7 @@
       </c>
       <c r="K48" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L48" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6722,7 +6722,7 @@
       </c>
       <c r="K49" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L49" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="K50" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L50" s="4" t="str">
         <f t="shared" si="7"/>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="K51" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L51" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7058,7 +7058,7 @@
       </c>
       <c r="K52" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L52" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7170,7 +7170,7 @@
       </c>
       <c r="K53" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L53" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="K54" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L54" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7400,7 +7400,7 @@
       </c>
       <c r="K55" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>0A</v>
+        <v>09</v>
       </c>
       <c r="L55" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="K56" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L56" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="K57" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>0A</v>
+        <v>09</v>
       </c>
       <c r="L57" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7742,7 +7742,7 @@
       </c>
       <c r="K58" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L58" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7851,7 +7851,7 @@
       </c>
       <c r="K59" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L59" s="4" t="str">
         <f t="shared" si="7"/>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="K60" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L60" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="K61" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L61" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8184,7 +8184,7 @@
       </c>
       <c r="K62" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L62" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="K63" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L63" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8408,7 +8408,7 @@
       </c>
       <c r="K64" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>0A</v>
+        <v>09</v>
       </c>
       <c r="L64" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8523,7 +8523,7 @@
       </c>
       <c r="K65" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L65" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8638,7 +8638,7 @@
       </c>
       <c r="K66" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>0A</v>
+        <v>09</v>
       </c>
       <c r="L66" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8753,7 +8753,7 @@
       </c>
       <c r="K67" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L67" s="4" t="str">
         <f t="shared" si="7"/>
@@ -8861,8 +8861,8 @@
         <v>02</v>
       </c>
       <c r="K68" s="4" t="str">
-        <f t="shared" ref="K68:K112" si="25">IF($G68="00",$G68,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G68)+1.669,0),2),2))</f>
-        <v>05</v>
+        <f t="shared" ref="K68:K112" si="25">IF($G68="00",$G68,DEC2HEX(MAX(ROUND(0.4145*HEX2DEC($G68)+0.669,0),1),2))</f>
+        <v>04</v>
       </c>
       <c r="L68" s="4" t="str">
         <f t="shared" ref="L68:L112" si="26">IF(OR($H68="7F",$H68="FF"),$H68,"00")</f>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="K69" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L69" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9086,7 +9086,7 @@
       </c>
       <c r="K70" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0C</v>
+        <v>0B</v>
       </c>
       <c r="L70" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9201,7 +9201,7 @@
       </c>
       <c r="K71" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L71" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="K72" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0C</v>
+        <v>0B</v>
       </c>
       <c r="L72" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="K73" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L73" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="K74" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L74" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="K75" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L75" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9764,7 +9764,7 @@
       </c>
       <c r="K76" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L76" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9879,7 +9879,7 @@
       </c>
       <c r="K77" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L77" s="4" t="str">
         <f t="shared" si="26"/>
@@ -9991,7 +9991,7 @@
       </c>
       <c r="K78" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L78" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10100,7 +10100,7 @@
       </c>
       <c r="K79" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L79" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10215,7 +10215,7 @@
       </c>
       <c r="K80" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0C</v>
+        <v>0B</v>
       </c>
       <c r="L80" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="K81" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0C</v>
+        <v>0B</v>
       </c>
       <c r="L81" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10445,7 +10445,7 @@
       </c>
       <c r="K82" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0B</v>
+        <v>0A</v>
       </c>
       <c r="L82" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="K83" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>10</v>
+        <v>0F</v>
       </c>
       <c r="L83" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10672,7 +10672,7 @@
       </c>
       <c r="K84" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0A</v>
+        <v>09</v>
       </c>
       <c r="L84" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10787,7 +10787,7 @@
       </c>
       <c r="K85" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L85" s="4" t="str">
         <f t="shared" si="26"/>
@@ -10896,7 +10896,7 @@
       </c>
       <c r="K86" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L86" s="4" t="str">
         <f t="shared" si="26"/>
@@ -11004,7 +11004,7 @@
       </c>
       <c r="K87" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L87" s="33" t="str">
         <f t="shared" si="26"/>
@@ -11118,7 +11118,7 @@
       </c>
       <c r="K88" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>10</v>
+        <v>0F</v>
       </c>
       <c r="L88" s="33" t="str">
         <f t="shared" si="26"/>
@@ -11232,7 +11232,7 @@
       </c>
       <c r="K89" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L89" s="33" t="str">
         <f t="shared" si="26"/>
@@ -11346,7 +11346,7 @@
       </c>
       <c r="K90" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>10</v>
+        <v>0F</v>
       </c>
       <c r="L90" s="33" t="str">
         <f t="shared" si="26"/>
@@ -11460,7 +11460,7 @@
       </c>
       <c r="K91" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L91" s="33" t="str">
         <f t="shared" si="26"/>
@@ -11575,7 +11575,7 @@
       </c>
       <c r="K92" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L92" s="4" t="str">
         <f t="shared" si="26"/>
@@ -11684,7 +11684,7 @@
       </c>
       <c r="K93" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L93" s="4" t="str">
         <f t="shared" si="26"/>
@@ -11793,7 +11793,7 @@
       </c>
       <c r="K94" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L94" s="4" t="str">
         <f t="shared" si="26"/>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="K95" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L95" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12011,7 +12011,7 @@
       </c>
       <c r="K96" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L96" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12120,7 +12120,7 @@
       </c>
       <c r="K97" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L97" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12229,7 +12229,7 @@
       </c>
       <c r="K98" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L98" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12338,7 +12338,7 @@
       </c>
       <c r="K99" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L99" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12447,7 +12447,7 @@
       </c>
       <c r="K100" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L100" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12562,7 +12562,7 @@
       </c>
       <c r="K101" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L101" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12677,7 +12677,7 @@
       </c>
       <c r="K102" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L102" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12792,7 +12792,7 @@
       </c>
       <c r="K103" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L103" s="4" t="str">
         <f t="shared" si="26"/>
@@ -12900,7 +12900,7 @@
       </c>
       <c r="K104" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0E</v>
+        <v>0D</v>
       </c>
       <c r="L104" s="33" t="str">
         <f t="shared" si="26"/>
@@ -13014,7 +13014,7 @@
       </c>
       <c r="K105" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L105" s="33" t="str">
         <f t="shared" si="26"/>
@@ -13128,7 +13128,7 @@
       </c>
       <c r="K106" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>10</v>
+        <v>0F</v>
       </c>
       <c r="L106" s="33" t="str">
         <f t="shared" si="26"/>
@@ -13242,7 +13242,7 @@
       </c>
       <c r="K107" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>0E</v>
+        <v>0D</v>
       </c>
       <c r="L107" s="33" t="str">
         <f t="shared" si="26"/>
@@ -13357,7 +13357,7 @@
       </c>
       <c r="K108" s="4" t="str">
         <f t="shared" si="25"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L108" s="4" t="str">
         <f t="shared" si="26"/>

</xml_diff>